<commit_message>
Upload pv_rcnn & pointpillar output files
</commit_message>
<xml_diff>
--- a/output/kitti_models/second/second_kitti_64_mean10.xlsx
+++ b/output/kitti_models/second/second_kitti_64_mean10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\half-beam\OpenPCDet\output\kitti_models\second\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{917799F6-169B-43EB-98C2-FE5B274CF1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E6BF74-26B5-49E1-9DCA-6BFC8F95286C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10569" yWindow="1277" windowWidth="17965" windowHeight="15540" xr2:uid="{6D827D38-8FA8-46F8-8899-41A9E871A376}"/>
+    <workbookView xWindow="630" yWindow="600" windowWidth="25755" windowHeight="12255" xr2:uid="{6D827D38-8FA8-46F8-8899-41A9E871A376}"/>
   </bookViews>
   <sheets>
     <sheet name="second_kitti_64_mean10" sheetId="1" r:id="rId1"/>
@@ -529,7 +529,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -623,8 +623,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Moderate_R40 Over # Beams Damaged</a:t>
+              <a:t>SECOND </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>On KITTI</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2585,7 +2590,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>